<commit_message>
looking at different curves fit
</commit_message>
<xml_diff>
--- a/b_fits_lm.xlsx
+++ b/b_fits_lm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jto208/Library/CloudStorage/OneDrive-UniversityofExeter/Pc paper/prochl_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7B5B2461-62D9-5342-AC1B-F97A72CC543F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AE8269BE-8D50-7443-9523-9EF2A38BC29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="21">
   <si>
     <t>d_name</t>
   </si>
@@ -958,15 +958,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H82"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H74" sqref="H74:H82"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -986,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1012,8 +1012,15 @@
         <f>RANK(F2,F2:F10,1)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <f>SUM(H6,H15,H24,H33,H42,H51,H60,H69,H78)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1039,8 +1046,15 @@
         <f>RANK(F3,F2:F10,1)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3">
+        <f>SUM(H8,H17,H26,H35,H44,H53,H62,H71,H80)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>19</v>
       </c>
@@ -1066,8 +1080,15 @@
         <f>RANK(F4,F2:F10,1)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <f>SUM(H2,H11,H20,H29,H38,H47,H56,H65,H74)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>28</v>
       </c>
@@ -1093,8 +1114,15 @@
         <f>RANK(F5,F2:F10,1)</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5">
+        <f>SUM(H9,H18,H27,H36,H45,H54,H63,H72,H81)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>37</v>
       </c>
@@ -1121,7 +1149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>46</v>
       </c>
@@ -1148,7 +1176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>55</v>
       </c>
@@ -1175,7 +1203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>64</v>
       </c>
@@ -1202,7 +1230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>73</v>
       </c>
@@ -1229,7 +1257,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1256,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1283,7 +1311,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
@@ -1310,7 +1338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>29</v>
       </c>
@@ -1337,7 +1365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>38</v>
       </c>
@@ -1364,7 +1392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>47</v>
       </c>
@@ -3186,7 +3214,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:G19"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>